<commit_message>
'TAWA_RTM.xlsx' had been updated
</commit_message>
<xml_diff>
--- a/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
+++ b/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="112">
   <si>
     <t>CR</t>
   </si>
@@ -52,10 +52,304 @@
     <t>TAWA_SIQ_009</t>
   </si>
   <si>
-    <t>FR-1</t>
-  </si>
-  <si>
-    <t>FR-2</t>
+    <t>TAWA_SIQ_012</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_016</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_017</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_018</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_019</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_020</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_021</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_029</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_030</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_031</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_032</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_042</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_001</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_038</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_002</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_003</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_004</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_005</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_006</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_007</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_008</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_009</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_010</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_011</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_012</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_013</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_014</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_015</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_016</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_017</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_018</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_019</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_020</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_021</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_022</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_023</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_024</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_025</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_026</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_027</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_028</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_029</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_030</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_031</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_032</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_033</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_034</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_035</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_036</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_037</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_039</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_040</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_041</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_042</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_046</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_047</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_048</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_049</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_050</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_051</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_052</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_053</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_054</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_005</t>
+  </si>
+  <si>
+    <t>………………………</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_055</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_033</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_056</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_057</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_058</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_059</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_060</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_061</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_062</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_063</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_064</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_065</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_066</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_067</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_068</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_069</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_070</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_071</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_072</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_073</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_074</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_075</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_076</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_077</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_078</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_079</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_080</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_081</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_043</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_082</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_084</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_085</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_086</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_087</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_089</t>
   </si>
 </sst>
 </file>
@@ -435,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,28 +777,691 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
+      <c r="C26" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
'TAWA_RTM.xlsx' document had been updated
</commit_message>
<xml_diff>
--- a/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
+++ b/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="193">
   <si>
     <t>CR</t>
   </si>
@@ -364,9 +364,6 @@
     <t>TAWA_WF_003</t>
   </si>
   <si>
-    <t>TAWA_CC_001</t>
-  </si>
-  <si>
     <t>TAWA_WF_007</t>
   </si>
   <si>
@@ -382,9 +379,6 @@
     <t>TAWA_SRS_NFR_002</t>
   </si>
   <si>
-    <t>TAWA_SIQ_002</t>
-  </si>
-  <si>
     <t>TAWA_SRS_FR_112</t>
   </si>
   <si>
@@ -412,9 +406,6 @@
     <t>TAWA_CR_005</t>
   </si>
   <si>
-    <t>TAWA_SIQ_011</t>
-  </si>
-  <si>
     <t>TAWA_SIQ_014</t>
   </si>
   <si>
@@ -511,9 +502,6 @@
     <t>TAWA_SIQ_038</t>
   </si>
   <si>
-    <t>TAWA_SIQ_040</t>
-  </si>
-  <si>
     <t>TAWA_SRS_FR_134</t>
   </si>
   <si>
@@ -542,6 +530,69 @@
   </si>
   <si>
     <t>TAWA_SRS_FR_125</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_039</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_093</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_094</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_095</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_096</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_098</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_104</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_106</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_107</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_108</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_115</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_118</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_127</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_128</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_130</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_047</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_132</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_137</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_140</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_141</t>
+  </si>
+  <si>
+    <t>TAWA_SRS_FR_142</t>
   </si>
 </sst>
 </file>
@@ -921,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,7 +1804,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>75</v>
@@ -1762,12 +1813,12 @@
         <v>76</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>75</v>
@@ -1776,12 +1827,12 @@
         <v>109</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>77</v>
@@ -1790,12 +1841,12 @@
         <v>78</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>77</v>
@@ -1804,12 +1855,12 @@
         <v>110</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>104</v>
@@ -1818,91 +1869,94 @@
         <v>105</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="D58" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>130</v>
+        <v>174</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -1910,10 +1964,10 @@
         <v>114</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>118</v>
+        <v>176</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>115</v>
@@ -1921,423 +1975,744 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E73"/>
+      <c r="F73"/>
+      <c r="G73"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E74"/>
+      <c r="F74"/>
+      <c r="G74"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E75"/>
+      <c r="F75"/>
+      <c r="G75"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="G76"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="D77" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="G77"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E79"/>
+      <c r="F79"/>
+      <c r="G79"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E81"/>
+      <c r="F81"/>
+      <c r="G81"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E82"/>
+      <c r="F82"/>
+      <c r="G82"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E83"/>
+      <c r="F83"/>
+      <c r="G83"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C68" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="D84" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E84"/>
+      <c r="F84"/>
+      <c r="G84"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="D85" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E85"/>
+      <c r="F85"/>
+      <c r="G85"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E86"/>
+      <c r="F86"/>
+      <c r="G86"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E87"/>
+      <c r="F87"/>
+      <c r="G87"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E88"/>
+      <c r="F88"/>
+      <c r="G88"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E89"/>
+      <c r="F89"/>
+      <c r="G89"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E90"/>
+      <c r="F90"/>
+      <c r="G90"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E92"/>
+      <c r="F92"/>
+      <c r="G92"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="C93" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E93"/>
+      <c r="F93"/>
+      <c r="G93"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E94"/>
+      <c r="F94"/>
+      <c r="G94"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C74" s="1" t="s">
+      <c r="D95" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E95"/>
+      <c r="F95"/>
+      <c r="G95"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E96"/>
+      <c r="F96"/>
+      <c r="G96"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E97"/>
+      <c r="F97"/>
+      <c r="G97"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E98"/>
+      <c r="F98"/>
+      <c r="G98"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E99"/>
+      <c r="F99"/>
+      <c r="G99"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E100"/>
+      <c r="F100"/>
+      <c r="G100"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E101"/>
+      <c r="F101"/>
+      <c r="G101"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E102"/>
+      <c r="F102"/>
+      <c r="G102"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E103"/>
+      <c r="F103"/>
+      <c r="G103"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E104"/>
+      <c r="F104"/>
+      <c r="G104"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E105"/>
+      <c r="F105"/>
+      <c r="G105"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="D106" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E106"/>
+      <c r="F106"/>
+      <c r="G106"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D79" s="1" t="s">
+      <c r="C107" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="E107"/>
+      <c r="F107"/>
+      <c r="G107"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="C108" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E108"/>
+      <c r="F108"/>
+      <c r="G108"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RTM design is updated
</commit_message>
<xml_diff>
--- a/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
+++ b/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="196">
   <si>
     <t>CR</t>
   </si>
@@ -593,6 +593,15 @@
   </si>
   <si>
     <t>TAWA_SRS_FR_142</t>
+  </si>
+  <si>
+    <t>Back End</t>
+  </si>
+  <si>
+    <t>Front End</t>
+  </si>
+  <si>
+    <t>Database</t>
   </si>
 </sst>
 </file>
@@ -629,7 +638,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -650,11 +659,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -666,6 +690,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -972,81 +1002,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>112</v>
       </c>
@@ -1054,33 +1088,33 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1088,16 +1122,16 @@
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1105,16 +1139,16 @@
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1122,16 +1156,16 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1139,16 +1173,16 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1156,16 +1190,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1173,16 +1207,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1190,16 +1224,16 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1207,16 +1241,16 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1224,16 +1258,16 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1241,16 +1275,16 @@
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1258,16 +1292,16 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I16" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1275,16 +1309,16 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I17" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1292,16 +1326,16 @@
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1309,30 +1343,33 @@
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1340,47 +1377,44 @@
         <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1388,16 +1422,16 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I24" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1405,30 +1439,33 @@
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="D26" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1436,13 +1473,13 @@
         <v>13</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1450,30 +1487,27 @@
         <v>13</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1481,16 +1515,16 @@
         <v>14</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I30" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1498,16 +1532,16 @@
         <v>14</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I31" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1515,16 +1549,16 @@
         <v>14</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I32" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1532,30 +1566,33 @@
         <v>14</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>114</v>
       </c>
@@ -1563,13 +1600,13 @@
         <v>15</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>114</v>
       </c>
@@ -1577,13 +1614,13 @@
         <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>114</v>
       </c>
@@ -1591,13 +1628,13 @@
         <v>15</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>114</v>
       </c>
@@ -1605,41 +1642,41 @@
         <v>15</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -1647,13 +1684,13 @@
         <v>17</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -1661,41 +1698,41 @@
         <v>17</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D44" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -1703,13 +1740,13 @@
         <v>19</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -1717,78 +1754,78 @@
         <v>19</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="D47" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G47" s="1" t="s">
+      <c r="D48" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G48" s="1" t="s">
+      <c r="D49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" s="1" t="s">
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G49" s="1" t="s">
+      <c r="D50" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>7</v>
       </c>
@@ -1796,27 +1833,27 @@
         <v>23</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>165</v>
       </c>
@@ -1824,27 +1861,27 @@
         <v>75</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>165</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>165</v>
       </c>
@@ -1852,58 +1889,58 @@
         <v>77</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>165</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>165</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E57"/>
-      <c r="F57"/>
-      <c r="G57"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>117</v>
       </c>
@@ -1911,27 +1948,27 @@
         <v>118</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>172</v>
+        <v>118</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>173</v>
+        <v>120</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>117</v>
       </c>
@@ -1939,41 +1976,41 @@
         <v>172</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>172</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>114</v>
       </c>
@@ -1981,13 +2018,13 @@
         <v>151</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>114</v>
       </c>
@@ -1995,13 +2032,13 @@
         <v>151</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>114</v>
       </c>
@@ -2009,55 +2046,55 @@
         <v>151</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>132</v>
+        <v>178</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>129</v>
       </c>
@@ -2068,10 +2105,10 @@
         <v>132</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>129</v>
       </c>
@@ -2082,44 +2119,41 @@
         <v>132</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>179</v>
+        <v>132</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E72"/>
-      <c r="F72"/>
-      <c r="G72"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="C73" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E73"/>
-      <c r="F73"/>
+        <v>159</v>
+      </c>
       <c r="G73"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73"/>
+      <c r="I73"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>117</v>
       </c>
@@ -2127,16 +2161,16 @@
         <v>136</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E74"/>
-      <c r="F74"/>
       <c r="G74"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74"/>
+      <c r="I74"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>117</v>
       </c>
@@ -2144,16 +2178,16 @@
         <v>136</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>137</v>
+        <v>181</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E75"/>
-      <c r="F75"/>
       <c r="G75"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75"/>
+      <c r="I75"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>117</v>
       </c>
@@ -2161,16 +2195,16 @@
         <v>136</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E76"/>
-      <c r="F76"/>
       <c r="G76"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76"/>
+      <c r="I76"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>117</v>
       </c>
@@ -2178,16 +2212,16 @@
         <v>136</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E77"/>
-      <c r="F77"/>
       <c r="G77"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77"/>
+      <c r="I77"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>117</v>
       </c>
@@ -2195,118 +2229,118 @@
         <v>136</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E78"/>
-      <c r="F78"/>
       <c r="G78"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78"/>
+      <c r="I78"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E79"/>
-      <c r="F79"/>
       <c r="G79"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79"/>
+      <c r="I79"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E80"/>
-      <c r="F80"/>
-      <c r="G80"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="G81"/>
+      <c r="H81"/>
+      <c r="I81"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E81"/>
-      <c r="F81"/>
-      <c r="G81"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="G82"/>
+      <c r="H82"/>
+      <c r="I82"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B83" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E82"/>
-      <c r="F82"/>
-      <c r="G82"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E83"/>
-      <c r="F83"/>
       <c r="G83"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83"/>
+      <c r="I83"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E84"/>
-      <c r="F84"/>
       <c r="G84"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84"/>
+      <c r="I84"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>126</v>
       </c>
@@ -2314,16 +2348,16 @@
         <v>140</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E85"/>
-      <c r="F85"/>
       <c r="G85"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85"/>
+      <c r="I85"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>126</v>
       </c>
@@ -2331,84 +2365,84 @@
         <v>140</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E86"/>
-      <c r="F86"/>
       <c r="G86"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86"/>
+      <c r="I86"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E87"/>
-      <c r="F87"/>
       <c r="G87"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87"/>
+      <c r="I87"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E88"/>
-      <c r="F88"/>
       <c r="G88"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88"/>
+      <c r="I88"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E89"/>
-      <c r="F89"/>
       <c r="G89"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89"/>
+      <c r="I89"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E90"/>
-      <c r="F90"/>
       <c r="G90"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90"/>
+      <c r="I90"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>126</v>
       </c>
@@ -2416,152 +2450,152 @@
         <v>127</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E91"/>
-      <c r="F91"/>
       <c r="G91"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91"/>
+      <c r="I91"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E92"/>
-      <c r="F92"/>
       <c r="G92"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92"/>
+      <c r="I92"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>123</v>
+        <v>161</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E93"/>
-      <c r="F93"/>
       <c r="G93"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93"/>
+      <c r="I93"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E94"/>
-      <c r="F94"/>
       <c r="G94"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94"/>
+      <c r="I94"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>128</v>
+        <v>186</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E95"/>
-      <c r="F95"/>
       <c r="G95"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95"/>
+      <c r="I95"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E96"/>
-      <c r="F96"/>
       <c r="G96"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96"/>
+      <c r="I96"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E97"/>
-      <c r="F97"/>
       <c r="G97"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97"/>
+      <c r="I97"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>117</v>
+        <v>168</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E98"/>
-      <c r="F98"/>
+        <v>125</v>
+      </c>
       <c r="G98"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98"/>
+      <c r="I98"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E99"/>
-      <c r="F99"/>
       <c r="G99"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99"/>
+      <c r="I99"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>129</v>
       </c>
@@ -2569,50 +2603,50 @@
         <v>157</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E100"/>
-      <c r="F100"/>
       <c r="G100"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100"/>
+      <c r="I100"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E101"/>
-      <c r="F101"/>
       <c r="G101"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101"/>
+      <c r="I101"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="C102" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E102"/>
-      <c r="F102"/>
+        <v>159</v>
+      </c>
       <c r="G102"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102"/>
+      <c r="I102"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>117</v>
       </c>
@@ -2620,16 +2654,16 @@
         <v>166</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E103"/>
-      <c r="F103"/>
       <c r="G103"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H103"/>
+      <c r="I103"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>117</v>
       </c>
@@ -2637,84 +2671,110 @@
         <v>166</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E104"/>
-      <c r="F104"/>
       <c r="G104"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104"/>
+      <c r="I104"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G105"/>
+      <c r="H105"/>
+      <c r="I105"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D106" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E105"/>
-      <c r="F105"/>
-      <c r="G105"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="G106"/>
+      <c r="H106"/>
+      <c r="I106"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B107" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C107" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E106"/>
-      <c r="F106"/>
-      <c r="G106"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="G107"/>
+      <c r="H107"/>
+      <c r="I107"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B108" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E107"/>
-      <c r="F107"/>
-      <c r="G107"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="G108"/>
+      <c r="H108"/>
+      <c r="I108"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C109" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D109" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E108"/>
-      <c r="F108"/>
-      <c r="G108"/>
+      <c r="G109"/>
+      <c r="H109"/>
+      <c r="I109"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Database is updated in RTM
</commit_message>
<xml_diff>
--- a/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
+++ b/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="213">
   <si>
     <t>CR</t>
   </si>
@@ -620,6 +620,43 @@
   </si>
   <si>
     <t>admin.php file &gt; (src="img/icons/edit.png")</t>
+  </si>
+  <si>
+    <t>TAWA_DB.USER</t>
+  </si>
+  <si>
+    <t>TAWA_DB.ADMIN</t>
+  </si>
+  <si>
+    <t>ــــ</t>
+  </si>
+  <si>
+    <t>TAWA_DB.TRAVEL
+TAWA_DB.HAS</t>
+  </si>
+  <si>
+    <t>TAWA_DB.ADD</t>
+  </si>
+  <si>
+    <t>TAWA_DB.FEEDBACK</t>
+  </si>
+  <si>
+    <t>TAWA_DB.TRAVEL
+TAWA_DB.VIEW</t>
+  </si>
+  <si>
+    <t>TAWA_DB.TRAVEL</t>
+  </si>
+  <si>
+    <t>TAWA_DB.BOOK</t>
+  </si>
+  <si>
+    <t>TAWA_DB.FEEDBACK
+TAWA_DB.ADD</t>
+  </si>
+  <si>
+    <t>TAWA_DB.USER
+TAWA_DB.MANAGE</t>
   </si>
 </sst>
 </file>
@@ -696,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -715,6 +752,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,66 +1065,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="24" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="5" t="s">
         <v>193</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1094,11 +1137,14 @@
       <c r="D3" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I3" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>112</v>
       </c>
@@ -1111,11 +1157,14 @@
       <c r="D4" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="I4" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>112</v>
       </c>
@@ -1128,11 +1177,14 @@
       <c r="D5" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I5" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1145,11 +1197,14 @@
       <c r="D6" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G6" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I6" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1162,11 +1217,14 @@
       <c r="D7" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I7" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1179,11 +1237,14 @@
       <c r="D8" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I8" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1196,11 +1257,14 @@
       <c r="D9" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I9" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1213,11 +1277,14 @@
       <c r="D10" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I10" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1230,11 +1297,14 @@
       <c r="D11" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I11" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1247,11 +1317,14 @@
       <c r="D12" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I12" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1264,11 +1337,14 @@
       <c r="D13" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I13" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1281,11 +1357,14 @@
       <c r="D14" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1298,11 +1377,14 @@
       <c r="D15" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I15" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1315,11 +1397,14 @@
       <c r="D16" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I16" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1332,11 +1417,14 @@
       <c r="D17" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I17" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1349,11 +1437,14 @@
       <c r="D18" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G18" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I18" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1366,11 +1457,14 @@
       <c r="D19" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I19" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -1383,11 +1477,14 @@
       <c r="D20" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="I20" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -1400,8 +1497,11 @@
       <c r="D21" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -1414,8 +1514,11 @@
       <c r="D22" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -1428,11 +1531,14 @@
       <c r="D23" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G23" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I23" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1445,11 +1551,14 @@
       <c r="D24" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I24" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1462,11 +1571,14 @@
       <c r="D25" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G25" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I25" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1479,11 +1591,14 @@
       <c r="D26" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G26" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I26" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1496,8 +1611,11 @@
       <c r="D27" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1510,8 +1628,11 @@
       <c r="D28" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -1524,8 +1645,11 @@
       <c r="D29" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -1538,11 +1662,14 @@
       <c r="D30" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G30" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="I30" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -1555,11 +1682,14 @@
       <c r="D31" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G31" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="I31" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1572,11 +1702,14 @@
       <c r="D32" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G32" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="I32" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1589,11 +1722,14 @@
       <c r="D33" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G33" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="I33" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1606,11 +1742,14 @@
       <c r="D34" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G34" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="I34" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>114</v>
       </c>
@@ -1623,8 +1762,11 @@
       <c r="D35" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>114</v>
       </c>
@@ -1637,8 +1779,11 @@
       <c r="D36" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G36" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>114</v>
       </c>
@@ -1651,8 +1796,11 @@
       <c r="D37" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>114</v>
       </c>
@@ -1665,8 +1813,11 @@
       <c r="D38" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G38" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>114</v>
       </c>
@@ -1679,8 +1830,11 @@
       <c r="D39" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>114</v>
       </c>
@@ -1693,8 +1847,11 @@
       <c r="D40" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G40" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -1707,8 +1864,11 @@
       <c r="D41" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -1721,8 +1881,11 @@
       <c r="D42" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G42" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -1735,8 +1898,11 @@
       <c r="D43" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G43" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -1749,8 +1915,11 @@
       <c r="D44" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G44" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>7</v>
       </c>
@@ -1763,8 +1932,11 @@
       <c r="D45" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G45" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -1777,8 +1949,11 @@
       <c r="D46" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G46" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -1791,8 +1966,11 @@
       <c r="D47" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G47" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -1805,11 +1983,14 @@
       <c r="D48" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G48" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I48" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>112</v>
       </c>
@@ -1822,11 +2003,14 @@
       <c r="D49" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G49" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I49" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>7</v>
       </c>
@@ -1839,11 +2023,14 @@
       <c r="D50" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="G50" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="I50" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>7</v>
       </c>
@@ -1856,8 +2043,11 @@
       <c r="D51" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G51" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>7</v>
       </c>
@@ -1870,8 +2060,11 @@
       <c r="D52" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G52" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>165</v>
       </c>
@@ -1887,8 +2080,11 @@
       <c r="F53" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G53" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>165</v>
       </c>
@@ -1904,8 +2100,11 @@
       <c r="F54" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G54" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>165</v>
       </c>
@@ -1921,8 +2120,11 @@
       <c r="F55" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G55" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>165</v>
       </c>
@@ -1938,8 +2140,11 @@
       <c r="F56" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G56" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>165</v>
       </c>
@@ -1955,8 +2160,11 @@
       <c r="F57" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G57" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>165</v>
       </c>
@@ -1972,11 +2180,13 @@
       <c r="F58" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G58"/>
+      <c r="G58" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H58"/>
       <c r="I58"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>117</v>
       </c>
@@ -1989,8 +2199,11 @@
       <c r="D59" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G59" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>117</v>
       </c>
@@ -2003,8 +2216,11 @@
       <c r="D60" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G60" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>117</v>
       </c>
@@ -2017,8 +2233,11 @@
       <c r="D61" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G61" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>117</v>
       </c>
@@ -2031,8 +2250,11 @@
       <c r="D62" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G62" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>114</v>
       </c>
@@ -2045,8 +2267,11 @@
       <c r="D63" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G63" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>114</v>
       </c>
@@ -2059,8 +2284,11 @@
       <c r="D64" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G64" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>114</v>
       </c>
@@ -2073,8 +2301,11 @@
       <c r="D65" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G65" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>114</v>
       </c>
@@ -2087,8 +2318,11 @@
       <c r="D66" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G66" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>114</v>
       </c>
@@ -2101,8 +2335,11 @@
       <c r="D67" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G67" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>114</v>
       </c>
@@ -2115,8 +2352,11 @@
       <c r="D68" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G68" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>129</v>
       </c>
@@ -2129,8 +2369,11 @@
       <c r="D69" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G69" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>129</v>
       </c>
@@ -2143,8 +2386,11 @@
       <c r="D70" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G70" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>129</v>
       </c>
@@ -2157,8 +2403,11 @@
       <c r="D71" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G71" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>129</v>
       </c>
@@ -2171,8 +2420,11 @@
       <c r="D72" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G72" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>129</v>
       </c>
@@ -2185,11 +2437,13 @@
       <c r="D73" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G73"/>
+      <c r="G73" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="H73"/>
       <c r="I73"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>117</v>
       </c>
@@ -2202,11 +2456,13 @@
       <c r="D74" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G74"/>
+      <c r="G74" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="H74"/>
       <c r="I74"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>117</v>
       </c>
@@ -2219,11 +2475,13 @@
       <c r="D75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G75"/>
+      <c r="G75" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="H75"/>
       <c r="I75"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>117</v>
       </c>
@@ -2236,11 +2494,13 @@
       <c r="D76" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G76"/>
+      <c r="G76" s="8" t="s">
+        <v>209</v>
+      </c>
       <c r="H76"/>
       <c r="I76"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>117</v>
       </c>
@@ -2253,11 +2513,13 @@
       <c r="D77" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G77"/>
+      <c r="G77" s="8" t="s">
+        <v>209</v>
+      </c>
       <c r="H77"/>
       <c r="I77"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>117</v>
       </c>
@@ -2270,11 +2532,13 @@
       <c r="D78" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G78"/>
+      <c r="G78" s="8" t="s">
+        <v>209</v>
+      </c>
       <c r="H78"/>
       <c r="I78"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>117</v>
       </c>
@@ -2287,11 +2551,13 @@
       <c r="D79" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G79"/>
+      <c r="G79" s="8" t="s">
+        <v>209</v>
+      </c>
       <c r="H79"/>
       <c r="I79"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>126</v>
       </c>
@@ -2304,11 +2570,13 @@
       <c r="D80" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G80"/>
+      <c r="G80" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H80"/>
       <c r="I80"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>126</v>
       </c>
@@ -2321,11 +2589,13 @@
       <c r="D81" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G81"/>
+      <c r="G81" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H81"/>
       <c r="I81"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>117</v>
       </c>
@@ -2338,11 +2608,13 @@
       <c r="D82" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G82"/>
+      <c r="G82" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H82"/>
       <c r="I82"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>129</v>
       </c>
@@ -2355,11 +2627,13 @@
       <c r="D83" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G83"/>
+      <c r="G83" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="H83"/>
       <c r="I83"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>126</v>
       </c>
@@ -2372,11 +2646,13 @@
       <c r="D84" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G84"/>
+      <c r="G84" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H84"/>
       <c r="I84"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>126</v>
       </c>
@@ -2389,11 +2665,13 @@
       <c r="D85" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G85"/>
+      <c r="G85" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H85"/>
       <c r="I85"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>126</v>
       </c>
@@ -2406,11 +2684,13 @@
       <c r="D86" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G86"/>
+      <c r="G86" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H86"/>
       <c r="I86"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>126</v>
       </c>
@@ -2423,11 +2703,13 @@
       <c r="D87" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G87"/>
+      <c r="G87" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H87"/>
       <c r="I87"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>122</v>
       </c>
@@ -2440,11 +2722,13 @@
       <c r="D88" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G88"/>
+      <c r="G88" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H88"/>
       <c r="I88"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>122</v>
       </c>
@@ -2457,11 +2741,13 @@
       <c r="D89" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G89"/>
+      <c r="G89" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H89"/>
       <c r="I89"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>126</v>
       </c>
@@ -2474,11 +2760,13 @@
       <c r="D90" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G90"/>
+      <c r="G90" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H90"/>
       <c r="I90"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>126</v>
       </c>
@@ -2491,11 +2779,13 @@
       <c r="D91" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G91"/>
+      <c r="G91" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H91"/>
       <c r="I91"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>126</v>
       </c>
@@ -2508,11 +2798,13 @@
       <c r="D92" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G92"/>
+      <c r="G92" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H92"/>
       <c r="I92"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>126</v>
       </c>
@@ -2525,11 +2817,13 @@
       <c r="D93" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G93"/>
+      <c r="G93" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H93"/>
       <c r="I93"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>126</v>
       </c>
@@ -2542,11 +2836,13 @@
       <c r="D94" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G94"/>
+      <c r="G94" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H94"/>
       <c r="I94"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>126</v>
       </c>
@@ -2559,11 +2855,13 @@
       <c r="D95" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G95"/>
+      <c r="G95" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H95"/>
       <c r="I95"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>126</v>
       </c>
@@ -2576,11 +2874,13 @@
       <c r="D96" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G96"/>
+      <c r="G96" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H96"/>
       <c r="I96"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>126</v>
       </c>
@@ -2593,11 +2893,13 @@
       <c r="D97" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G97"/>
+      <c r="G97" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H97"/>
       <c r="I97"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>126</v>
       </c>
@@ -2610,11 +2912,13 @@
       <c r="D98" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G98"/>
+      <c r="G98" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H98"/>
       <c r="I98"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>129</v>
       </c>
@@ -2627,11 +2931,13 @@
       <c r="D99" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G99"/>
+      <c r="G99" s="8" t="s">
+        <v>211</v>
+      </c>
       <c r="H99"/>
       <c r="I99"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>129</v>
       </c>
@@ -2644,11 +2950,13 @@
       <c r="D100" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G100"/>
+      <c r="G100" s="8" t="s">
+        <v>211</v>
+      </c>
       <c r="H100"/>
       <c r="I100"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>129</v>
       </c>
@@ -2661,11 +2969,13 @@
       <c r="D101" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G101"/>
+      <c r="G101" s="8" t="s">
+        <v>211</v>
+      </c>
       <c r="H101"/>
       <c r="I101"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>129</v>
       </c>
@@ -2678,11 +2988,13 @@
       <c r="D102" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G102"/>
+      <c r="G102" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H102"/>
       <c r="I102"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>117</v>
       </c>
@@ -2698,11 +3010,13 @@
       <c r="F103" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G103"/>
+      <c r="G103" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="H103"/>
       <c r="I103"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>117</v>
       </c>
@@ -2718,11 +3032,13 @@
       <c r="F104" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G104"/>
+      <c r="G104" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="H104"/>
       <c r="I104"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>117</v>
       </c>
@@ -2738,11 +3054,13 @@
       <c r="F105" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G105"/>
+      <c r="G105" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="H105"/>
       <c r="I105"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>117</v>
       </c>
@@ -2755,11 +3073,13 @@
       <c r="D106" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G106"/>
+      <c r="G106" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="H106"/>
       <c r="I106"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>122</v>
       </c>
@@ -2772,11 +3092,13 @@
       <c r="D107" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G107"/>
+      <c r="G107" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H107"/>
       <c r="I107"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>114</v>
       </c>
@@ -2789,11 +3111,13 @@
       <c r="D108" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G108"/>
+      <c r="G108" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="H108"/>
       <c r="I108"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>117</v>
       </c>
@@ -2806,7 +3130,9 @@
       <c r="D109" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G109"/>
+      <c r="G109" s="8" t="s">
+        <v>205</v>
+      </c>
       <c r="H109"/>
       <c r="I109"/>
     </row>

</xml_diff>

<commit_message>
Add home and destination modules
</commit_message>
<xml_diff>
--- a/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
+++ b/Requirements/Technical Requirements/Traceability Matrix/TAWA_RTM.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$170</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$170</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="344">
   <si>
     <t>CR</t>
   </si>
@@ -1027,6 +1027,49 @@
   </si>
   <si>
     <t>TAWA_SignUp_052</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAWA_HomePage_004 
+TAWA_HomePage_005
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+TAWA_HomePage_006
+</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_007</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_008</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_010</t>
+  </si>
+  <si>
+    <t>TAWA_HomePage_013</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_001</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_002</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_003</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_004</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_005</t>
+  </si>
+  <si>
+    <t>TAWA_Destination_006</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1187,11 +1230,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1201,6 +1244,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1509,8 +1558,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C68" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="G132" workbookViewId="0">
+      <selection activeCell="H132" sqref="H132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,16 +1576,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
@@ -1544,18 +1593,18 @@
       </c>
       <c r="F1" s="17"/>
       <c r="G1" s="18"/>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="5" t="s">
         <v>191</v>
       </c>
@@ -1565,10 +1614,10 @@
       <c r="G2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1591,7 +1640,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>110</v>
       </c>
@@ -1614,7 +1663,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>110</v>
       </c>
@@ -1637,7 +1686,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>110</v>
       </c>
@@ -1660,7 +1709,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1686,7 +1735,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1710,7 +1759,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>163</v>
       </c>
@@ -1734,7 +1783,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1760,7 +1809,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1786,7 +1835,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1812,7 +1861,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1838,7 +1887,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -1864,7 +1913,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1890,7 +1939,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -1916,7 +1965,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1939,7 +1988,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
@@ -1965,7 +2014,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1991,7 +2040,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -2017,7 +2066,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -2043,7 +2092,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -2069,7 +2118,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>7</v>
       </c>
@@ -2095,7 +2144,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
@@ -2121,7 +2170,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>7</v>
       </c>
@@ -2147,7 +2196,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -2173,7 +2222,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -2199,7 +2248,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -2225,7 +2274,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
@@ -2251,7 +2300,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>7</v>
       </c>
@@ -2277,7 +2326,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>7</v>
       </c>
@@ -2303,7 +2352,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -2329,7 +2378,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -2355,7 +2404,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -2381,7 +2430,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2407,7 +2456,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -2433,7 +2482,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -2459,7 +2508,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -2485,7 +2534,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -2511,7 +2560,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -2537,7 +2586,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -2563,7 +2612,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2589,7 +2638,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>7</v>
       </c>
@@ -2608,7 +2657,7 @@
       <c r="G43" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="H43" s="15" t="s">
+      <c r="H43" s="14" t="s">
         <v>213</v>
       </c>
       <c r="I43" s="1" t="s">
@@ -2661,7 +2710,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -2687,7 +2736,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>7</v>
       </c>
@@ -2713,7 +2762,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="12.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>7</v>
       </c>
@@ -2739,7 +2788,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="12.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>7</v>
       </c>
@@ -2765,7 +2814,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>7</v>
       </c>
@@ -2791,7 +2840,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>7</v>
       </c>
@@ -2817,7 +2866,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>7</v>
       </c>
@@ -2866,7 +2915,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>7</v>
       </c>
@@ -2892,7 +2941,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>7</v>
       </c>
@@ -2918,7 +2967,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>7</v>
       </c>
@@ -2944,7 +2993,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>7</v>
       </c>
@@ -2970,7 +3019,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>7</v>
       </c>
@@ -2996,7 +3045,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>7</v>
       </c>
@@ -3022,7 +3071,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>7</v>
       </c>
@@ -3048,7 +3097,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>7</v>
       </c>
@@ -3074,7 +3123,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>7</v>
       </c>
@@ -3100,7 +3149,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>7</v>
       </c>
@@ -3126,7 +3175,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>7</v>
       </c>
@@ -3152,7 +3201,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>7</v>
       </c>
@@ -3178,7 +3227,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>7</v>
       </c>
@@ -3204,7 +3253,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>7</v>
       </c>
@@ -3230,7 +3279,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>7</v>
       </c>
@@ -3256,7 +3305,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>7</v>
       </c>
@@ -3282,7 +3331,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>7</v>
       </c>
@@ -3308,7 +3357,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>7</v>
       </c>
@@ -3334,7 +3383,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>112</v>
       </c>
@@ -3353,8 +3402,11 @@
       <c r="G72" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H72" s="19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>112</v>
       </c>
@@ -3373,8 +3425,11 @@
       <c r="G73" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H73" s="20" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>112</v>
       </c>
@@ -3393,8 +3448,11 @@
       <c r="G74" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H74" s="20" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>112</v>
       </c>
@@ -3413,8 +3471,9 @@
       <c r="G75" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H75" s="20"/>
+    </row>
+    <row r="76" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>112</v>
       </c>
@@ -3434,7 +3493,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>112</v>
       </c>
@@ -3523,7 +3582,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>7</v>
       </c>
@@ -3549,7 +3608,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>7</v>
       </c>
@@ -3575,7 +3634,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>7</v>
       </c>
@@ -3601,7 +3660,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>7</v>
       </c>
@@ -3627,7 +3686,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>7</v>
       </c>
@@ -3653,7 +3712,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>7</v>
       </c>
@@ -3679,7 +3738,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>7</v>
       </c>
@@ -3705,7 +3764,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>7</v>
       </c>
@@ -3728,7 +3787,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>7</v>
       </c>
@@ -3751,7 +3810,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>7</v>
       </c>
@@ -3774,7 +3833,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>7</v>
       </c>
@@ -3797,7 +3856,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>7</v>
       </c>
@@ -3820,7 +3879,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>110</v>
       </c>
@@ -3843,7 +3902,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>110</v>
       </c>
@@ -3866,7 +3925,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>110</v>
       </c>
@@ -3882,14 +3941,14 @@
       <c r="G95" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H95" s="15" t="s">
+      <c r="H95" s="14" t="s">
         <v>215</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>7</v>
       </c>
@@ -3908,14 +3967,14 @@
       <c r="G96" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H96" s="15" t="s">
+      <c r="H96" s="14" t="s">
         <v>216</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>7</v>
       </c>
@@ -3938,7 +3997,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>7</v>
       </c>
@@ -3961,7 +4020,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>7</v>
       </c>
@@ -4197,7 +4256,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>112</v>
       </c>
@@ -4213,8 +4272,11 @@
       <c r="G110" s="7" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H110" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>112</v>
       </c>
@@ -4233,8 +4295,11 @@
       <c r="G111" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H111" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>112</v>
       </c>
@@ -4253,8 +4318,11 @@
       <c r="G112" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H112" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
@@ -4274,7 +4342,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
@@ -4294,7 +4362,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>112</v>
       </c>
@@ -4331,7 +4399,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>127</v>
       </c>
@@ -4351,7 +4419,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>127</v>
       </c>
@@ -4413,7 +4481,7 @@
       <c r="H120"/>
       <c r="I120"/>
     </row>
-    <row r="121" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>115</v>
       </c>
@@ -4432,10 +4500,12 @@
       <c r="G121" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="H121"/>
+      <c r="H121" t="s">
+        <v>337</v>
+      </c>
       <c r="I121"/>
     </row>
-    <row r="122" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>115</v>
       </c>
@@ -4454,10 +4524,12 @@
       <c r="G122" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="H122"/>
+      <c r="H122" t="s">
+        <v>337</v>
+      </c>
       <c r="I122"/>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>115</v>
       </c>
@@ -4476,10 +4548,12 @@
       <c r="G123" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="H123"/>
+      <c r="H123" t="s">
+        <v>338</v>
+      </c>
       <c r="I123"/>
     </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>115</v>
       </c>
@@ -4498,10 +4572,12 @@
       <c r="G124" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="H124"/>
+      <c r="H124" t="s">
+        <v>339</v>
+      </c>
       <c r="I124"/>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>115</v>
       </c>
@@ -4517,10 +4593,12 @@
       <c r="G125" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="H125"/>
+      <c r="H125" t="s">
+        <v>340</v>
+      </c>
       <c r="I125"/>
     </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>115</v>
       </c>
@@ -4539,10 +4617,12 @@
       <c r="G126" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="H126"/>
+      <c r="H126" t="s">
+        <v>341</v>
+      </c>
       <c r="I126"/>
     </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>124</v>
       </c>
@@ -4561,10 +4641,12 @@
       <c r="G127" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="H127"/>
+      <c r="H127" t="s">
+        <v>342</v>
+      </c>
       <c r="I127"/>
     </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>124</v>
       </c>
@@ -4583,10 +4665,12 @@
       <c r="G128" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="H128"/>
+      <c r="H128" t="s">
+        <v>343</v>
+      </c>
       <c r="I128"/>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>115</v>
       </c>
@@ -4605,7 +4689,9 @@
       <c r="G129" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="H129"/>
+      <c r="H129" t="s">
+        <v>341</v>
+      </c>
       <c r="I129"/>
     </row>
     <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -4630,7 +4716,7 @@
       <c r="H130"/>
       <c r="I130"/>
     </row>
-    <row r="131" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>124</v>
       </c>
@@ -4651,7 +4737,7 @@
       </c>
       <c r="I131"/>
     </row>
-    <row r="132" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>124</v>
       </c>
@@ -4672,7 +4758,7 @@
       </c>
       <c r="I132"/>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>124</v>
       </c>
@@ -4693,7 +4779,7 @@
       </c>
       <c r="I133"/>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>124</v>
       </c>
@@ -4714,7 +4800,7 @@
       </c>
       <c r="I134"/>
     </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>120</v>
       </c>
@@ -4735,7 +4821,7 @@
       </c>
       <c r="I135"/>
     </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>120</v>
       </c>
@@ -4756,7 +4842,7 @@
       </c>
       <c r="I136"/>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>124</v>
       </c>
@@ -4777,7 +4863,7 @@
       </c>
       <c r="I137"/>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>124</v>
       </c>
@@ -4798,7 +4884,7 @@
       </c>
       <c r="I138"/>
     </row>
-    <row r="139" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>124</v>
       </c>
@@ -4819,7 +4905,7 @@
       </c>
       <c r="I139"/>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>124</v>
       </c>
@@ -4840,7 +4926,7 @@
       </c>
       <c r="I140"/>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>124</v>
       </c>
@@ -4861,7 +4947,7 @@
       </c>
       <c r="I141"/>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>124</v>
       </c>
@@ -4882,7 +4968,7 @@
       </c>
       <c r="I142"/>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>124</v>
       </c>
@@ -4903,7 +4989,7 @@
       </c>
       <c r="I143"/>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>124</v>
       </c>
@@ -4924,7 +5010,7 @@
       </c>
       <c r="I144"/>
     </row>
-    <row r="145" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>124</v>
       </c>
@@ -5105,7 +5191,7 @@
       </c>
       <c r="I152"/>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>115</v>
       </c>
@@ -5124,7 +5210,7 @@
       <c r="H153"/>
       <c r="I153"/>
     </row>
-    <row r="154" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>120</v>
       </c>
@@ -5145,7 +5231,7 @@
       </c>
       <c r="I154"/>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>112</v>
       </c>
@@ -5164,7 +5250,7 @@
       <c r="H155"/>
       <c r="I155"/>
     </row>
-    <row r="156" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>115</v>
       </c>
@@ -5404,12 +5490,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D170">
-    <filterColumn colId="0">
+  <autoFilter ref="A1:I170">
+    <filterColumn colId="3">
       <filters>
-        <filter val="TAWA_WF_001"/>
+        <filter val="TAWA_WF_003"/>
+        <filter val="TAWA_WF_004"/>
+        <filter val="TAWA_WF_005"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="4" showButton="0"/>
+    <filterColumn colId="5" showButton="0"/>
   </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="I1:I2"/>

</xml_diff>